<commit_message>
Cronograma, gráfica de global cost
* Gráfica de global cost ya bonita
</commit_message>
<xml_diff>
--- a/Inteligencia Computacional/Documentos/Cronograma-tesis-bonito.xlsx
+++ b/Inteligencia Computacional/Documentos/Cronograma-tesis-bonito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaby\Documents\UVG\5A2S\tesis\git-tesis\Inteligencia Computacional\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4397D8AD-9296-481C-AC30-93C5127C8DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50844112-2FB4-44F8-A6AF-374FA4BD757E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -607,6 +607,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -618,39 +651,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1064,7 +1064,7 @@
   <dimension ref="A1:BO30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="H3" sqref="H3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1111,37 +1111,37 @@
         <v>26</v>
       </c>
       <c r="H2" s="13">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="14"/>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="35"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="33" t="s">
+      <c r="Q2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="35"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="31"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="36" t="s">
+      <c r="V2" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="38"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="34"/>
       <c r="Z2" s="17"/>
-      <c r="AA2" s="27" t="s">
+      <c r="AA2" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="29"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="40"/>
       <c r="AE2" s="18"/>
       <c r="AF2" s="22" t="s">
         <v>37</v>
@@ -1156,57 +1156,57 @@
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="1:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30" t="s">
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30" t="s">
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30" t="s">
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="30"/>
-      <c r="Z3" s="30" t="s">
+      <c r="W3" s="41"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="30"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="41"/>
       <c r="AE3" s="20" t="s">
         <v>32</v>
       </c>
@@ -1219,12 +1219,12 @@
       <c r="AL3" s="19"/>
     </row>
     <row r="4" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="40"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -2029,6 +2029,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="M3:P3"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:T2"/>
@@ -2038,12 +2044,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="M3:P3"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO30">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
PRM, tesis, cronograma y algunas imágenes
Además, se removió el archivo params ev, ya que ahora es obsoleto.
</commit_message>
<xml_diff>
--- a/Inteligencia Computacional/Documentos/Cronograma-tesis-bonito.xlsx
+++ b/Inteligencia Computacional/Documentos/Cronograma-tesis-bonito.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaby\Documents\UVG\5A2S\tesis\git-tesis\Inteligencia Computacional\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50844112-2FB4-44F8-A6AF-374FA4BD757E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9300E9-D91B-421B-B040-30F8E0706D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1063,8 +1063,8 @@
   </sheetPr>
   <dimension ref="A1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:L3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1111,7 +1111,7 @@
         <v>26</v>
       </c>
       <c r="H2" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J2" s="14"/>
       <c r="K2" s="29" t="s">
@@ -1925,10 +1925,10 @@
         <v>12</v>
       </c>
       <c r="F26" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G26" s="8">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.25" hidden="1" x14ac:dyDescent="0.3">

</xml_diff>